<commit_message>
just working on stuff!
</commit_message>
<xml_diff>
--- a/Global Competitiveness Index/data18.xlsx
+++ b/Global Competitiveness Index/data18.xlsx
@@ -6238,7 +6238,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1.0900000000000001</t>
+          <t>1.09</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1.1000000000000001</t>
+          <t>1.10</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -7156,7 +7156,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1.1100000000000001</t>
+          <t>1.11</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -7615,7 +7615,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1.1200000000000001</t>
+          <t>1.12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -8533,7 +8533,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1.1299999999999999</t>
+          <t>1.13</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -8992,7 +8992,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1.1399999999999999</t>
+          <t>1.14</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -9451,7 +9451,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1.1499999999999999</t>
+          <t>1.15</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -9910,7 +9910,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1.1599999999999999</t>
+          <t>1.16</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -13123,7 +13123,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>1.20</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -15418,7 +15418,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2.0099999999999998</t>
+          <t>2.01</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -16336,7 +16336,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2.0299999999999998</t>
+          <t>2.03</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -17146,7 +17146,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2.0499999999999998</t>
+          <t>2.05</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -18523,7 +18523,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2.0699999999999998</t>
+          <t>2.07</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -23566,7 +23566,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4.0199999999999996</t>
+          <t>4.02</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -25201,7 +25201,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>4.0599999999999996</t>
+          <t>4.06</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -27874,7 +27874,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4.0999999999999996</t>
+          <t>4.10</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -30151,7 +30151,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>5.0199999999999996</t>
+          <t>5.02</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -32437,7 +32437,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>5.0599999999999996</t>
+          <t>5.06</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -41617,7 +41617,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>6.10</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -49414,7 +49414,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>7.10</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -51706,7 +51706,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>8.0299999999999994</t>
+          <t>8.03</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -52165,7 +52165,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>8.0399999999999991</t>
+          <t>8.04</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -52624,7 +52624,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>8.0500000000000007</t>
+          <t>8.05</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -56755,7 +56755,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>9.0299999999999994</t>
+          <t>9.03</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -57673,7 +57673,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>9.0399999999999991</t>
+          <t>9.04</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -58132,7 +58132,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>9.0500000000000007</t>
+          <t>9.05</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -60427,7 +60427,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>10.029999999999999</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -60886,7 +60886,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>10.039999999999999</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -72355,7 +72355,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>GCI</t>
+          <t>Glob</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">

</xml_diff>